<commit_message>
Control de cambios versión 2
</commit_message>
<xml_diff>
--- a/Desarrollo/SGEH/Fuentes/SGEH-DEC.xlsx
+++ b/Desarrollo/SGEH/Fuentes/SGEH-DEC.xlsx
@@ -8,15 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\UNMSM\CICLO VI\GCS-WONG\Estado de Cambio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC454966-70A4-4911-88C5-E3D5FAAE5756}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4BB598-418E-48EA-A08E-57C97C7F6CB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Estados de Solicitud de Cambio" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mgpXwrv42td76QbkWjxKitpKvM/vw=="/>
     </ext>
@@ -25,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -102,10 +111,40 @@
     <t>La solicitud de cambio ha sido desaprobada por el comité de control de cambios.</t>
   </si>
   <si>
+    <t>Planificado</t>
+  </si>
+  <si>
+    <t>Se ha realizado la planificación de actividades que se describe en la solicitud de cambio emitida por el usuario.</t>
+  </si>
+  <si>
+    <t>Archivado</t>
+  </si>
+  <si>
+    <t>La solicitud de cambio se archiva por encargado de gestión de cambios</t>
+  </si>
+  <si>
+    <t>Implementado</t>
+  </si>
+  <si>
+    <t>Se ha implementado la solicitud de cambio emitida por el usuario.</t>
+  </si>
+  <si>
+    <t>Verificado</t>
+  </si>
+  <si>
+    <t>El usuario ha verificado la funcionalidad del cambio.</t>
+  </si>
+  <si>
+    <t>Terminado</t>
+  </si>
+  <si>
+    <t>La solicitud de cambio se da por terminado.</t>
+  </si>
+  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>ESTADOS DE SOLICITUD DE CAMBIOS</t>
+    <t>ESTADOS DE SOLICITUD DE CAMBIO</t>
   </si>
 </sst>
 </file>
@@ -188,7 +227,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -286,11 +325,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF674EA7"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF674EA7"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF674EA7"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF674EA7"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF674EA7"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -343,6 +427,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -564,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:J1002"/>
+  <dimension ref="B1:K1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
@@ -587,27 +683,27 @@
     <col min="15" max="26" width="9.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="14.4">
+    <row r="1" spans="2:11" ht="14.4">
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="2:10" ht="46.5" customHeight="1">
+    <row r="2" spans="2:11" ht="46.5" customHeight="1">
       <c r="B2" s="1"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="2:10" ht="48" customHeight="1">
-      <c r="B3" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="F3" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="2:11" ht="48" customHeight="1" thickBot="1">
+      <c r="B3" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="3"/>
       <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="2:10" ht="35.25" customHeight="1">
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="2:11" ht="35.25" customHeight="1" thickBot="1">
       <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
@@ -617,10 +713,10 @@
       <c r="D4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="2:10" ht="72" customHeight="1">
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="2:11" ht="72" customHeight="1" thickBot="1">
       <c r="B5" s="7">
         <v>1</v>
       </c>
@@ -630,10 +726,10 @@
       <c r="D5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="2:10" ht="69.75" customHeight="1">
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="2:11" ht="69.75" customHeight="1" thickBot="1">
       <c r="B6" s="10">
         <v>2</v>
       </c>
@@ -643,10 +739,10 @@
       <c r="D6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="2:10" ht="72" customHeight="1">
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="2:11" ht="72" customHeight="1" thickBot="1">
       <c r="B7" s="13">
         <v>3</v>
       </c>
@@ -657,10 +753,10 @@
         <v>8</v>
       </c>
       <c r="E7" s="16"/>
-      <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="2:10" ht="66.75" customHeight="1">
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="2:11" ht="66.75" customHeight="1" thickBot="1">
       <c r="B8" s="17">
         <v>4</v>
       </c>
@@ -670,10 +766,10 @@
       <c r="D8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="2:10" ht="73.5" customHeight="1">
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="2:11" ht="73.5" customHeight="1" thickBot="1">
       <c r="B9" s="13">
         <v>5</v>
       </c>
@@ -683,13 +779,13 @@
       <c r="D9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="2:10" ht="73.5" customHeight="1">
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="2:11" ht="73.5" customHeight="1" thickBot="1">
       <c r="B10" s="17">
         <v>6</v>
       </c>
@@ -699,13 +795,13 @@
       <c r="D10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="2:10" ht="73.5" customHeight="1">
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="2:11" ht="73.5" customHeight="1" thickBot="1">
       <c r="B11" s="13">
         <v>7</v>
       </c>
@@ -715,13 +811,13 @@
       <c r="D11" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="2:10" ht="80.25" customHeight="1">
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="2:11" ht="80.25" customHeight="1" thickBot="1">
       <c r="B12" s="17">
         <v>8</v>
       </c>
@@ -731,13 +827,13 @@
       <c r="D12" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="2:10" ht="73.5" customHeight="1">
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="2:11" ht="73.5" customHeight="1" thickBot="1">
       <c r="B13" s="13">
         <v>9</v>
       </c>
@@ -747,13 +843,13 @@
       <c r="D13" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="2:10" ht="67.5" customHeight="1">
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="2:11" ht="67.5" customHeight="1" thickBot="1">
       <c r="B14" s="17">
         <v>10</v>
       </c>
@@ -763,13 +859,13 @@
       <c r="D14" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="2:10" ht="57" customHeight="1">
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="2:11" ht="57" customHeight="1" thickBot="1">
       <c r="B15" s="13">
         <v>11</v>
       </c>
@@ -779,59 +875,107 @@
       <c r="D15" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="2:10" ht="69" customHeight="1">
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="2:11" ht="69" customHeight="1" thickBot="1">
+      <c r="B16" s="17">
+        <v>12</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="2:7" ht="72" customHeight="1">
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="2:11" ht="72" customHeight="1" thickBot="1">
+      <c r="B17" s="13">
+        <v>13</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>28</v>
+      </c>
       <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="2:7" ht="75" customHeight="1"/>
-    <row r="19" spans="2:7" ht="57" customHeight="1"/>
-    <row r="20" spans="2:7" ht="60" customHeight="1"/>
-    <row r="21" spans="2:7" ht="60.75" customHeight="1"/>
-    <row r="22" spans="2:7" ht="14.4">
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="2:11" ht="75" customHeight="1" thickBot="1">
+      <c r="B18" s="17">
+        <v>14</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" ht="57" customHeight="1" thickBot="1">
+      <c r="B19" s="13">
+        <v>15</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="60" customHeight="1" thickBot="1">
+      <c r="B20" s="21">
+        <v>16</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" ht="60.75" customHeight="1"/>
+    <row r="22" spans="2:11" ht="14.4">
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="2:7" ht="15.75" customHeight="1">
+    <row r="23" spans="2:11" ht="15.75" customHeight="1">
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="2:7" ht="15.75" customHeight="1">
+    <row r="24" spans="2:11" ht="15.75" customHeight="1">
       <c r="B24" s="1"/>
     </row>
-    <row r="25" spans="2:7" ht="15.75" customHeight="1">
+    <row r="25" spans="2:11" ht="15.75" customHeight="1">
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="2:7" ht="15.75" customHeight="1">
+    <row r="26" spans="2:11" ht="15.75" customHeight="1">
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="2:7" ht="15.75" customHeight="1">
+    <row r="27" spans="2:11" ht="15.75" customHeight="1">
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="2:7" ht="15.75" customHeight="1">
+    <row r="28" spans="2:11" ht="15.75" customHeight="1">
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="2:7" ht="15.75" customHeight="1">
+    <row r="29" spans="2:11" ht="15.75" customHeight="1">
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="2:7" ht="15.75" customHeight="1">
+    <row r="30" spans="2:11" ht="15.75" customHeight="1">
       <c r="F30" s="16"/>
     </row>
-    <row r="31" spans="2:7" ht="15.75" customHeight="1"/>
-    <row r="32" spans="2:7" ht="15.75" customHeight="1"/>
+    <row r="31" spans="2:11" ht="15.75" customHeight="1"/>
+    <row r="32" spans="2:11" ht="15.75" customHeight="1"/>
     <row r="33" spans="2:5" ht="43.5" customHeight="1"/>
     <row r="34" spans="2:5" ht="43.5" customHeight="1"/>
     <row r="35" spans="2:5" ht="43.5" customHeight="1"/>
@@ -843,7 +987,7 @@
     <row r="39" spans="2:5" ht="27.75" customHeight="1"/>
     <row r="40" spans="2:5" ht="54.75" customHeight="1">
       <c r="E40" s="16" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="2:5" ht="54.75" customHeight="1"/>

</xml_diff>

<commit_message>
Control de cambios versión 3
</commit_message>
<xml_diff>
--- a/Desarrollo/SGEH/Fuentes/SGEH-DEC.xlsx
+++ b/Desarrollo/SGEH/Fuentes/SGEH-DEC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\UNMSM\CICLO VI\GCS-WONG\Estado de Cambio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4BB598-418E-48EA-A08E-57C97C7F6CB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68DCD0C-0F59-4D35-9132-AE8FAABD2947}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
+  <si>
+    <t>NIVELES DE URGENCIA</t>
+  </si>
   <si>
     <t>ID</t>
   </si>
@@ -45,28 +48,56 @@
     <t>Descripción</t>
   </si>
   <si>
+    <t>Nombre</t>
+  </si>
+  <si>
     <t>Creado</t>
   </si>
   <si>
     <t>El usuario ha creado la solicitud de cambios.</t>
   </si>
   <si>
+    <t>Bajo</t>
+  </si>
+  <si>
+    <t>El cambio es requerido para implementar mejoras o liberar nuevas versiones planeadas de los servicios.</t>
+  </si>
+  <si>
     <t>Recibido</t>
   </si>
   <si>
     <t>El sistema de gestión de cambios recepciona y lista solicitud de cambios.</t>
   </si>
   <si>
+    <t>Medio</t>
+  </si>
+  <si>
+    <t>El cambio es requerido para implementar ajustes funcionales en los servicios.</t>
+  </si>
+  <si>
     <t>Revisado</t>
   </si>
   <si>
     <t>El encargado de gestión de cambios verifica que solicitud de cambios cumpla con formato establecido</t>
   </si>
   <si>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>El cambio es requerido para corregir un error que está generando indisponibilidad parcial de los servicios</t>
+  </si>
+  <si>
     <t>Rechazado - Tipo 1</t>
   </si>
   <si>
     <t>El encargado de gestión de cambios rechaza solicitud de cambios porque no cumple con formato establecido</t>
+  </si>
+  <si>
+    <t>Crítica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El cambio es requerido para habilitar o restaurar los servicios.
+</t>
   </si>
   <si>
     <t>Asignado</t>
@@ -195,7 +226,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,6 +237,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF674EA7"/>
         <bgColor rgb="FF674EA7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF741B47"/>
+        <bgColor rgb="FF741B47"/>
       </patternFill>
     </fill>
     <fill>
@@ -222,12 +259,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFEAD1DC"/>
+        <bgColor rgb="FFEAD1DC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFDFDFD"/>
         <bgColor rgb="FFFDFDFD"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -281,23 +324,53 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF674EA7"/>
+      <left style="thick">
+        <color rgb="FF741B47"/>
       </left>
-      <right style="medium">
+      <right style="thick">
         <color rgb="FFFFFFFF"/>
       </right>
-      <top style="medium">
-        <color rgb="FFFFFFFF"/>
+      <top style="thick">
+        <color rgb="FF741B47"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thick">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF741B47"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF741B47"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF741B47"/>
+      </top>
+      <bottom style="thick">
         <color rgb="FFFFFFFF"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FF674EA7"/>
       </left>
       <right style="medium">
         <color rgb="FFFFFFFF"/>
@@ -315,6 +388,21 @@
         <color rgb="FFFFFFFF"/>
       </left>
       <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
         <color rgb="FF674EA7"/>
       </right>
       <top style="medium">
@@ -322,6 +410,96 @@
       </top>
       <bottom style="medium">
         <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF741B47"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF741B47"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF741B47"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF741B47"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF741B47"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF741B47"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF741B47"/>
       </bottom>
       <diagonal/>
     </border>
@@ -374,7 +552,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -392,44 +570,13 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -439,6 +586,76 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -660,10 +877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K1002"/>
+  <dimension ref="B1:N1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
@@ -683,101 +900,151 @@
     <col min="15" max="26" width="9.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="14.4">
+    <row r="1" spans="2:14" ht="14.4">
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="2:11" ht="46.5" customHeight="1">
+    <row r="2" spans="2:14" ht="46.5" customHeight="1">
       <c r="B2" s="1"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="2:11" ht="48" customHeight="1" thickBot="1">
-      <c r="B3" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="3"/>
+    <row r="3" spans="2:14" ht="48" customHeight="1" thickBot="1">
+      <c r="B3" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="G3" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="2:11" ht="35.25" customHeight="1" thickBot="1">
+      <c r="L3" s="3"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="2:14" ht="35.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="B4" s="4" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="H4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="2:14" ht="72" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B5" s="10">
+        <v>1</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="13">
+        <v>1</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="2:14" ht="69.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B6" s="16">
         <v>2</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="2:11" ht="72" customHeight="1" thickBot="1">
-      <c r="B5" s="7">
-        <v>1</v>
-      </c>
-      <c r="C5" s="8" t="s">
+      <c r="C6" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="19">
+        <v>2</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="2:14" ht="72" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B7" s="22">
         <v>3</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="C7" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="25"/>
+      <c r="G7" s="26">
+        <v>3</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="2:14" ht="66.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B8" s="27">
         <v>4</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="2:11" ht="69.75" customHeight="1" thickBot="1">
-      <c r="B6" s="10">
-        <v>2</v>
-      </c>
-      <c r="C6" s="11" t="s">
+      <c r="C8" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="29">
+        <v>4</v>
+      </c>
+      <c r="H8" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="2:14" ht="73.5" customHeight="1" thickBot="1">
+      <c r="B9" s="22">
         <v>5</v>
       </c>
-      <c r="D6" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="2:11" ht="72" customHeight="1" thickBot="1">
-      <c r="B7" s="13">
-        <v>3</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="16"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="2:11" ht="66.75" customHeight="1" thickBot="1">
-      <c r="B8" s="17">
-        <v>4</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="2:11" ht="73.5" customHeight="1" thickBot="1">
-      <c r="B9" s="13">
-        <v>5</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>12</v>
+      <c r="C9" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>22</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -785,15 +1052,15 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="2:11" ht="73.5" customHeight="1" thickBot="1">
-      <c r="B10" s="17">
+    <row r="10" spans="2:14" ht="73.5" customHeight="1" thickBot="1">
+      <c r="B10" s="27">
         <v>6</v>
       </c>
-      <c r="C10" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>14</v>
+      <c r="C10" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>24</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -801,15 +1068,15 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="2:11" ht="73.5" customHeight="1" thickBot="1">
-      <c r="B11" s="13">
+    <row r="11" spans="2:14" ht="73.5" customHeight="1" thickBot="1">
+      <c r="B11" s="22">
         <v>7</v>
       </c>
-      <c r="C11" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>16</v>
+      <c r="C11" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>26</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -817,15 +1084,15 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="2:11" ht="80.25" customHeight="1" thickBot="1">
-      <c r="B12" s="17">
+    <row r="12" spans="2:14" ht="80.25" customHeight="1" thickBot="1">
+      <c r="B12" s="27">
         <v>8</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>18</v>
+      <c r="C12" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>28</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -833,15 +1100,15 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="2:11" ht="73.5" customHeight="1" thickBot="1">
-      <c r="B13" s="13">
+    <row r="13" spans="2:14" ht="73.5" customHeight="1" thickBot="1">
+      <c r="B13" s="22">
         <v>9</v>
       </c>
-      <c r="C13" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>20</v>
+      <c r="C13" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>30</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -849,133 +1116,133 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="2:11" ht="67.5" customHeight="1" thickBot="1">
-      <c r="B14" s="17">
+    <row r="14" spans="2:14" ht="67.5" customHeight="1" thickBot="1">
+      <c r="B14" s="27">
         <v>10</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>22</v>
-      </c>
+      <c r="C14" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-    </row>
-    <row r="15" spans="2:11" ht="57" customHeight="1" thickBot="1">
-      <c r="B15" s="13">
+    </row>
+    <row r="15" spans="2:14" ht="57" customHeight="1" thickBot="1">
+      <c r="B15" s="22">
         <v>11</v>
       </c>
-      <c r="C15" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>24</v>
-      </c>
+      <c r="C15" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-    </row>
-    <row r="16" spans="2:11" ht="69" customHeight="1" thickBot="1">
-      <c r="B16" s="17">
+    </row>
+    <row r="16" spans="2:14" ht="69" customHeight="1" thickBot="1">
+      <c r="B16" s="27">
         <v>12</v>
       </c>
-      <c r="C16" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>26</v>
-      </c>
+      <c r="C16" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="2:11" ht="72" customHeight="1" thickBot="1">
-      <c r="B17" s="13">
+    </row>
+    <row r="17" spans="2:10" ht="72" customHeight="1" thickBot="1">
+      <c r="B17" s="22">
         <v>13</v>
       </c>
-      <c r="C17" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="C17" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-    </row>
-    <row r="18" spans="2:11" ht="75" customHeight="1" thickBot="1">
-      <c r="B18" s="17">
+    </row>
+    <row r="18" spans="2:10" ht="75" customHeight="1" thickBot="1">
+      <c r="B18" s="27">
         <v>14</v>
       </c>
-      <c r="C18" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" ht="57" customHeight="1" thickBot="1">
-      <c r="B19" s="13">
+      <c r="C18" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="57" customHeight="1" thickBot="1">
+      <c r="B19" s="22">
         <v>15</v>
       </c>
-      <c r="C19" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" ht="60" customHeight="1" thickBot="1">
-      <c r="B20" s="21">
+      <c r="C19" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="33" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" ht="60" customHeight="1" thickBot="1">
+      <c r="B20" s="34">
         <v>16</v>
       </c>
-      <c r="C20" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="23" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" ht="60.75" customHeight="1"/>
-    <row r="22" spans="2:11" ht="14.4">
+      <c r="C20" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="36" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="60.75" customHeight="1"/>
+    <row r="22" spans="2:10" ht="14.4">
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="2:11" ht="15.75" customHeight="1">
+    <row r="23" spans="2:10" ht="15.75" customHeight="1">
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="2:11" ht="15.75" customHeight="1">
+    <row r="24" spans="2:10" ht="15.75" customHeight="1">
       <c r="B24" s="1"/>
     </row>
-    <row r="25" spans="2:11" ht="15.75" customHeight="1">
+    <row r="25" spans="2:10" ht="15.75" customHeight="1">
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="2:11" ht="15.75" customHeight="1">
+    <row r="26" spans="2:10" ht="15.75" customHeight="1">
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="2:11" ht="15.75" customHeight="1">
+    <row r="27" spans="2:10" ht="15.75" customHeight="1">
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="2:11" ht="15.75" customHeight="1">
+    <row r="28" spans="2:10" ht="15.75" customHeight="1">
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="2:11" ht="15.75" customHeight="1">
+    <row r="29" spans="2:10" ht="15.75" customHeight="1">
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="2:11" ht="15.75" customHeight="1">
-      <c r="F30" s="16"/>
-    </row>
-    <row r="31" spans="2:11" ht="15.75" customHeight="1"/>
-    <row r="32" spans="2:11" ht="15.75" customHeight="1"/>
+    <row r="30" spans="2:10" ht="15.75" customHeight="1">
+      <c r="F30" s="25"/>
+    </row>
+    <row r="31" spans="2:10" ht="15.75" customHeight="1"/>
+    <row r="32" spans="2:10" ht="15.75" customHeight="1"/>
     <row r="33" spans="2:5" ht="43.5" customHeight="1"/>
     <row r="34" spans="2:5" ht="43.5" customHeight="1"/>
     <row r="35" spans="2:5" ht="43.5" customHeight="1"/>
@@ -986,8 +1253,8 @@
     <row r="38" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="39" spans="2:5" ht="27.75" customHeight="1"/>
     <row r="40" spans="2:5" ht="54.75" customHeight="1">
-      <c r="E40" s="16" t="s">
-        <v>35</v>
+      <c r="E40" s="25" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="2:5" ht="54.75" customHeight="1"/>
@@ -3851,7 +4118,8 @@
       <c r="B1002" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="G3:I3"/>
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
Correción versión DEC final
</commit_message>
<xml_diff>
--- a/Desarrollo/SGEH/Fuentes/SGEH-DEC.xlsx
+++ b/Desarrollo/SGEH/Fuentes/SGEH-DEC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\UNMSM\CICLO VI\GCS-WONG\Estado de Cambio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D551299-C4BE-4DA5-ADE4-A918514A6FDD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21811CD5-3774-4AB7-8466-776E7496E353}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Estados de Solicitud de Cambio" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="105">
   <si>
     <t>NIVELES DE URGENCIA</t>
   </si>
@@ -322,6 +322,24 @@
   </si>
   <si>
     <t>Fecha de inicio en que se empezó el cambio</t>
+  </si>
+  <si>
+    <t>Se detalla la Fecha de finalización del cambio</t>
+  </si>
+  <si>
+    <t>Persona que se encargó de pasar la solicitud de cambio</t>
+  </si>
+  <si>
+    <t>Fecha de recepción del cambio</t>
+  </si>
+  <si>
+    <t>Fecha en la que se implementó el cambio</t>
+  </si>
+  <si>
+    <t>Fecha en la que se verificó el cambio</t>
+  </si>
+  <si>
+    <t>El nombre del usuario que verificó</t>
   </si>
   <si>
     <t xml:space="preserve">ESTADO DE SOLICITUD DE CAMBIOS </t>
@@ -335,7 +353,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -409,6 +427,12 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Comfortaa"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Comfortaa"/>
     </font>
   </fonts>
@@ -510,7 +534,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="47">
+  <borders count="49">
     <border>
       <left/>
       <right/>
@@ -1202,11 +1226,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF6AA84F"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF6AA84F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF6AA84F"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF6AA84F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1489,6 +1543,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="16" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1712,7 +1778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:N1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -1742,16 +1808,16 @@
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="2:14" ht="48" customHeight="1">
-      <c r="B3" s="98" t="s">
-        <v>98</v>
-      </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="G3" s="98" t="s">
+      <c r="B3" s="102" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="103"/>
+      <c r="D3" s="103"/>
+      <c r="G3" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
+      <c r="H3" s="103"/>
+      <c r="I3" s="103"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="4"/>
@@ -1879,11 +1945,11 @@
       <c r="D9" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="98" t="s">
+      <c r="G9" s="102" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="99"/>
-      <c r="I9" s="99"/>
+      <c r="H9" s="103"/>
+      <c r="I9" s="103"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
@@ -2000,11 +2066,11 @@
       <c r="D14" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="G14" s="98" t="s">
+      <c r="G14" s="102" t="s">
         <v>40</v>
       </c>
-      <c r="H14" s="99"/>
-      <c r="I14" s="99"/>
+      <c r="H14" s="103"/>
+      <c r="I14" s="103"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
@@ -6339,10 +6405,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8343DFC-08AC-4800-88E9-DDAD0E61B053}">
-  <dimension ref="B2:C21"/>
+  <dimension ref="B2:C22"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8"/>
@@ -6456,12 +6522,55 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="2:3" ht="72.599999999999994" customHeight="1" thickTop="1"/>
-    <row r="17" ht="61.8" customHeight="1"/>
-    <row r="18" ht="57.6" customHeight="1"/>
-    <row r="19" ht="71.400000000000006" customHeight="1"/>
-    <row r="20" ht="71.400000000000006" customHeight="1"/>
-    <row r="21" ht="58.2" customHeight="1"/>
+    <row r="16" spans="2:3" ht="72.599999999999994" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B16" s="98" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="95" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="61.8" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B17" s="99" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="97" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="57.6" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B18" s="98" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="95" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="71.400000000000006" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B19" s="99" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" s="97" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="71.400000000000006" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B20" s="98" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="95" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="58.2" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B21" s="100" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" s="101" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="14.4" thickTop="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Corrección DEC versión final (#80)
* Creacion BD

* Diagrama de clases y Modelo Logico BD

* Correción documentos

* Correccion de nomenclatura y Diagrama de clases

* PI Avance 5

* Mt version 4

* Documento de registro de pruebas version final

* Correción versión DEC final
</commit_message>
<xml_diff>
--- a/Desarrollo/SGEH/Fuentes/SGEH-DEC.xlsx
+++ b/Desarrollo/SGEH/Fuentes/SGEH-DEC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\UNMSM\CICLO VI\GCS-WONG\Estado de Cambio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D551299-C4BE-4DA5-ADE4-A918514A6FDD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21811CD5-3774-4AB7-8466-776E7496E353}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Estados de Solicitud de Cambio" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="105">
   <si>
     <t>NIVELES DE URGENCIA</t>
   </si>
@@ -322,6 +322,24 @@
   </si>
   <si>
     <t>Fecha de inicio en que se empezó el cambio</t>
+  </si>
+  <si>
+    <t>Se detalla la Fecha de finalización del cambio</t>
+  </si>
+  <si>
+    <t>Persona que se encargó de pasar la solicitud de cambio</t>
+  </si>
+  <si>
+    <t>Fecha de recepción del cambio</t>
+  </si>
+  <si>
+    <t>Fecha en la que se implementó el cambio</t>
+  </si>
+  <si>
+    <t>Fecha en la que se verificó el cambio</t>
+  </si>
+  <si>
+    <t>El nombre del usuario que verificó</t>
   </si>
   <si>
     <t xml:space="preserve">ESTADO DE SOLICITUD DE CAMBIOS </t>
@@ -335,7 +353,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -409,6 +427,12 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Comfortaa"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Comfortaa"/>
     </font>
   </fonts>
@@ -510,7 +534,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="47">
+  <borders count="49">
     <border>
       <left/>
       <right/>
@@ -1202,11 +1226,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF6AA84F"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF6AA84F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF6AA84F"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF6AA84F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1489,6 +1543,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="16" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1712,7 +1778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:N1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -1742,16 +1808,16 @@
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="2:14" ht="48" customHeight="1">
-      <c r="B3" s="98" t="s">
-        <v>98</v>
-      </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="G3" s="98" t="s">
+      <c r="B3" s="102" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="103"/>
+      <c r="D3" s="103"/>
+      <c r="G3" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
+      <c r="H3" s="103"/>
+      <c r="I3" s="103"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="4"/>
@@ -1879,11 +1945,11 @@
       <c r="D9" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="98" t="s">
+      <c r="G9" s="102" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="99"/>
-      <c r="I9" s="99"/>
+      <c r="H9" s="103"/>
+      <c r="I9" s="103"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
@@ -2000,11 +2066,11 @@
       <c r="D14" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="G14" s="98" t="s">
+      <c r="G14" s="102" t="s">
         <v>40</v>
       </c>
-      <c r="H14" s="99"/>
-      <c r="I14" s="99"/>
+      <c r="H14" s="103"/>
+      <c r="I14" s="103"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
@@ -6339,10 +6405,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8343DFC-08AC-4800-88E9-DDAD0E61B053}">
-  <dimension ref="B2:C21"/>
+  <dimension ref="B2:C22"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8"/>
@@ -6456,12 +6522,55 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="2:3" ht="72.599999999999994" customHeight="1" thickTop="1"/>
-    <row r="17" ht="61.8" customHeight="1"/>
-    <row r="18" ht="57.6" customHeight="1"/>
-    <row r="19" ht="71.400000000000006" customHeight="1"/>
-    <row r="20" ht="71.400000000000006" customHeight="1"/>
-    <row r="21" ht="58.2" customHeight="1"/>
+    <row r="16" spans="2:3" ht="72.599999999999994" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B16" s="98" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="95" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="61.8" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B17" s="99" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="97" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="57.6" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B18" s="98" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="95" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="71.400000000000006" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B19" s="99" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" s="97" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="71.400000000000006" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B20" s="98" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="95" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="58.2" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B21" s="100" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" s="101" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="14.4" thickTop="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>